<commit_message>
Thêm ảnh product và detail, xửa file exel
</commit_message>
<xml_diff>
--- a/CuaHangTrangSuc/productsInfo/products.xlsx
+++ b/CuaHangTrangSuc/productsInfo/products.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767E5DC4-516D-4CA7-B552-1E1D7549AFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67551777-6B89-4CB5-A37D-CBC58F7F7F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="243">
   <si>
     <t>ID</t>
   </si>
@@ -1588,6 +1588,262 @@
   </si>
   <si>
     <t>Đồng Hồ Orient Nam SUNE5002W0 Dây Thép Không Gỉ 41mm</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng 10K PNJ dây đan kiểu chữ cong 0000W000105</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-trang-10k-8094.html</t>
+  </si>
+  <si>
+    <r>
+      <t>1.080.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GD0000W000105</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng 10K PNJ 0000W000220</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-trang-10k-gdmrwkxx025.006.html</t>
+  </si>
+  <si>
+    <r>
+      <t>1.322.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GD0000W000220</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-vang-trang-10k-6813.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng 10K PNJ 0000W000177</t>
+  </si>
+  <si>
+    <r>
+      <t>1.717.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t> GD0000W000177</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-vang-18k-6555.html?</t>
+  </si>
+  <si>
+    <r>
+      <t>2.341.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng 18K PNJ kiểu dây đan dập chữ S xoắn suốt 0000Y000711</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-trang-y-18k-8727.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng Ý 18K PNJ 0000W000277</t>
+  </si>
+  <si>
+    <r>
+      <t>2.175.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng 18K PNJ dây đan kiểu chữ cong 0000Y000256</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-18k-day-dan-kieu-chu-cong-vi.html</t>
+  </si>
+  <si>
+    <r>
+      <t>1.862.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GD0000Y000256</t>
+  </si>
+  <si>
+    <t>GD0000W000277</t>
+  </si>
+  <si>
+    <t>GD0000Y000711</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-vang-18k-dinh-da-cz-7256.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K đính đá CZ PNJ XMXMY000021</t>
+  </si>
+  <si>
+    <t>GCXMXMY000021</t>
+  </si>
+  <si>
+    <r>
+      <t>6.713.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-vang-18k-dinh-da-cz-ya59993.102.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K đính đá CZ PNJ XMXMY000019</t>
+  </si>
+  <si>
+    <r>
+      <t>6.627.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GCXMXMY000019</t>
   </si>
 </sst>
 </file>
@@ -2016,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3300,68 +3556,164 @@
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="27.6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
+      <c r="B82" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="E82" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
+      <c r="B83" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="E83" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F83" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
+      <c r="B84" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="E84" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F84" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
+      <c r="B85" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="E85" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F85" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
+      <c r="B86" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="E86" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
+      <c r="B87" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>231</v>
+      </c>
       <c r="E87" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
+      <c r="B88" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="E88" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
+      <c r="B89" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="E89" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="F89" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update ảnh sản phẩm
</commit_message>
<xml_diff>
--- a/CuaHangTrangSuc/productsInfo/products.xlsx
+++ b/CuaHangTrangSuc/productsInfo/products.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EA85-DF56-404F-950D-CF93E6DC4426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="334">
   <si>
     <t>ID</t>
   </si>
@@ -2374,12 +2375,364 @@
   </si>
   <si>
     <t>https://www.pnj.com.vn/dong-ho-skagen-nu-skw2799-day-thep-khong-gi-25mm.html?gender=female&amp;category=dong-ho_dong-ho-skagen</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-vang-18k-dinh-da-cz-ya81532.102.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K đính đá CZ PNJ XMXMY000026</t>
+  </si>
+  <si>
+    <r>
+      <t>20.615.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GCXMXMY000026</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-sac-xuan-vang-trang-14k-dinh-da-topaz-95249.600.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng trắng 14K đính đá Topaz PNJ Sắc Xuân TPMXW000003</t>
+  </si>
+  <si>
+    <r>
+      <t>9.275.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GCTPMXW000003</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-sac-xuan-18k-vang-dinh-da-citrine-yb88479.600.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K Vàng đính đá Citrine PNJ Sắc Xuân CTXMY000004</t>
+  </si>
+  <si>
+    <t>GCCTXMY000004</t>
+  </si>
+  <si>
+    <r>
+      <t>10.326.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-phuong-hoang-vang-18k-dinh-da-ruby-81993.600.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K đính đá Ruby PNJ Phượng Hoàng RBXMY000016</t>
+  </si>
+  <si>
+    <r>
+      <t>10.691.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GCRBXMY000016</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-vang-trang-14k-dinh-da-topaz-79812.600.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng trắng 14K đính đá Topaz PNJ TPXMW000005</t>
+  </si>
+  <si>
+    <r>
+      <t>68.528.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GCTPXMW000005</t>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-pnj-sac-xuan-vang-18k-dinh-da-citrine-yb88324.600.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng 18K Vàng đính đá Citrine PNJ Sắc Xuân CTXMY000003</t>
+  </si>
+  <si>
+    <t>GCCTXMY000003</t>
+  </si>
+  <si>
+    <r>
+      <t>10.342.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-18k-8738.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng 18K PNJ 0000Y000952</t>
+  </si>
+  <si>
+    <t>GD0000Y000952</t>
+  </si>
+  <si>
+    <r>
+      <t>2.441.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-vang-10k-6920.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng 10K PNJ kiểu dây đan lật đôi 0000W000221</t>
+  </si>
+  <si>
+    <t>GD0000W000221</t>
+  </si>
+  <si>
+    <r>
+      <t>1.826.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-pnj-vang-18k-8750.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng 18K PNJ 0000Y000708</t>
+  </si>
+  <si>
+    <t>GD0000Y000708</t>
+  </si>
+  <si>
+    <r>
+      <t>2.450.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-chuyen-vang-trang-18k-pnj-0000w060032.html</t>
+  </si>
+  <si>
+    <t>Dây chuyền Vàng trắng 18K PNJ 0000W060032</t>
+  </si>
+  <si>
+    <t>GD0000W060032</t>
+  </si>
+  <si>
+    <r>
+      <t>10.346.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.pnj.com.vn/day-co-vang-y-18k-pnj-0000h060001.html</t>
+  </si>
+  <si>
+    <t>Dây cổ Vàng Ý 18K PNJ 0000H060001</t>
+  </si>
+  <si>
+    <r>
+      <t>5.723.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color rgb="FFBB934D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+  </si>
+  <si>
+    <t>GC0000H060001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2565,6 +2918,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2600,6 +2970,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2775,11 +3162,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4281,7 +4668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4289,7 +4676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4297,7 +4684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4305,7 +4692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4313,7 +4700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4321,7 +4708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4329,7 +4716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4337,7 +4724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4345,7 +4732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4353,7 +4740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4361,103 +4748,235 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
+      <c r="B91" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="E91" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
+      <c r="B92" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>296</v>
+      </c>
       <c r="E92" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
+      <c r="B93" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="E93" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="21" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
+      <c r="B94" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>304</v>
+      </c>
       <c r="E94" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
+      <c r="B95" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>308</v>
+      </c>
       <c r="E95" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
+      <c r="B96" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="E96" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
+      <c r="B97" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="E97" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="27.6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
+      <c r="B98" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>321</v>
+      </c>
       <c r="E98" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>325</v>
+      </c>
       <c r="E99" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
+      <c r="B100" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>329</v>
+      </c>
       <c r="E100" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
+      <c r="B101" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>332</v>
+      </c>
       <c r="E101" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="F101" t="s">
+        <v>330</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F38" r:id="rId6"/>
-    <hyperlink ref="F50" r:id="rId7"/>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F38" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F50" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>